<commit_message>
rough draft of paper
</commit_message>
<xml_diff>
--- a/survey/surveydata.xlsx
+++ b/survey/surveydata.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10958"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10958" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Survey Responses" sheetId="1" r:id="rId1"/>
+    <sheet name="Topic Subjects" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,39 +25,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Respondent Name</t>
-  </si>
-  <si>
-    <t>Topic 1</t>
-  </si>
-  <si>
-    <t>Topic 2</t>
-  </si>
-  <si>
-    <t>Topic 3</t>
-  </si>
-  <si>
-    <t>Topic 4</t>
-  </si>
-  <si>
-    <t>Topic 5</t>
-  </si>
-  <si>
-    <t>Topic 6</t>
-  </si>
-  <si>
-    <t>Topic 7</t>
-  </si>
-  <si>
-    <t>Topic 8</t>
-  </si>
-  <si>
-    <t>Topic 9</t>
-  </si>
-  <si>
-    <t>Topic 10</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+  <si>
+    <t>Topic1</t>
+  </si>
+  <si>
+    <t>Topic2</t>
+  </si>
+  <si>
+    <t>Topic3</t>
+  </si>
+  <si>
+    <t>Topic4</t>
+  </si>
+  <si>
+    <t>Topic5</t>
+  </si>
+  <si>
+    <t>Topic6</t>
+  </si>
+  <si>
+    <t>Topic7</t>
+  </si>
+  <si>
+    <t>Topic8</t>
+  </si>
+  <si>
+    <t>Topic9</t>
+  </si>
+  <si>
+    <t>Topic10</t>
+  </si>
+  <si>
+    <t>RespondentID</t>
+  </si>
+  <si>
+    <t>Availability during production failures</t>
+  </si>
+  <si>
+    <t>Financial incentives in the supply chain</t>
+  </si>
+  <si>
+    <t>Assessing competing products</t>
+  </si>
+  <si>
+    <t>Safety and effectiveness</t>
+  </si>
+  <si>
+    <t>Co-ordination of government financing programs</t>
+  </si>
+  <si>
+    <t>Payment for vaccination and follow up care</t>
+  </si>
+  <si>
+    <t>Side Effect monitoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bioterrorism </t>
+  </si>
+  <si>
+    <t>Communicating Risks and improving knowledge</t>
+  </si>
+  <si>
+    <t>Global Health</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>subject</t>
   </si>
 </sst>
 </file>
@@ -410,46 +447,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.265625" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -716,6 +755,112 @@
       </c>
       <c r="G20">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed colours for respondents with zero satisfaction
</commit_message>
<xml_diff>
--- a/survey/surveydata.xlsx
+++ b/survey/surveydata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10958" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10958"/>
   </bookViews>
   <sheets>
     <sheet name="Survey Responses" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Topic1</t>
   </si>
@@ -94,6 +94,63 @@
   </si>
   <si>
     <t>subject</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -447,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -492,8 +549,8 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>23</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -506,8 +563,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>24</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -520,8 +577,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>25</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -534,8 +591,8 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>4</v>
+      <c r="A5" t="s">
+        <v>26</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -548,8 +605,8 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>5</v>
+      <c r="A6" t="s">
+        <v>27</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -562,8 +619,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>28</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -576,8 +633,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>29</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -590,8 +647,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>8</v>
+      <c r="A9" t="s">
+        <v>30</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -604,8 +661,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>9</v>
+      <c r="A10" t="s">
+        <v>31</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -618,8 +675,8 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>10</v>
+      <c r="A11" t="s">
+        <v>32</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -632,8 +689,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>33</v>
       </c>
       <c r="I12">
         <v>3</v>
@@ -646,8 +703,8 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>12</v>
+      <c r="A13" t="s">
+        <v>34</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -660,8 +717,8 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>13</v>
+      <c r="A14" t="s">
+        <v>35</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -674,8 +731,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>36</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -688,8 +745,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>37</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -702,8 +759,8 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>38</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -716,8 +773,8 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>39</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -730,8 +787,8 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A19">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>40</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -744,8 +801,8 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A20">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>41</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -766,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>